<commit_message>
Inscription + login + article public + mes articles + navigation topic a gauche + recherche d'un template adapter pour le profile
</commit_message>
<xml_diff>
--- a/Divers/Planification.xlsx
+++ b/Divers/Planification.xlsx
@@ -563,7 +563,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="40">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -622,6 +622,13 @@
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1154,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,67 +2719,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F54:F56 C52:C58 G52:G58 I52:I53 E52:E58 L52:L58 D57 C28:C50 D32 E25:E50 I25:I50 L25:L48 C25:C26 H54:I55 I56:I58 K56 C2:M24 G25:G37 G39:G50 F38 L50">
-    <cfRule type="cellIs" dxfId="38" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:M37 C52:M55 D27:M27 C28:M34 C26:M26 C57:M58 C56:G56 I56:M56 C2:M24 C39:M48 H38:M38 C38:F38 C50:M50 C49:J49 L49:M49">
-    <cfRule type="cellIs" dxfId="37" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51 I51 G51 E51 C51">
-    <cfRule type="cellIs" dxfId="36" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="15" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:M51">
-    <cfRule type="cellIs" dxfId="35" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:K57 F57 H57 M57">
-    <cfRule type="cellIs" dxfId="34" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="13" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54:D56 G54:G56 J54:K55 J56">
-    <cfRule type="cellIs" dxfId="33" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="12" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:M27 C28:M37 C57:M58 C56:G56 I56:M56 C2:M26 C39:M48 H38:M38 C38:F38 C50:M55 C49:J49 L49:M49">
-    <cfRule type="cellIs" dxfId="32" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N58">
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:M59">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2786,7 +2793,7 @@
   <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="O60" sqref="O60"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3159,7 +3166,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4">
-        <v>1.0416666666666666E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -3171,7 +3178,7 @@
       <c r="M14" s="23"/>
       <c r="N14" s="3">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3184,7 +3191,7 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -3196,7 +3203,7 @@
       <c r="M15" s="23"/>
       <c r="N15" s="3">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3333,9 +3340,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4">
+      <c r="F21" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="I21" s="4"/>
@@ -3358,9 +3363,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4">
+      <c r="F22" s="4">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I22" s="4"/>
@@ -3384,12 +3387,11 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="4">
-        <v>4.1666666666666664E-2</v>
-      </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="23"/>
@@ -3409,12 +3411,11 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="G24" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="4">
-        <v>4.1666666666666664E-2</v>
-      </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="23"/>
@@ -3474,11 +3475,10 @@
         <v>3.125E-2</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="F27" s="13"/>
-      <c r="G27" s="4">
-        <v>3.125E-2</v>
-      </c>
       <c r="H27" s="13"/>
       <c r="I27" s="4"/>
       <c r="J27" s="13"/>
@@ -3487,7 +3487,7 @@
       <c r="M27" s="15"/>
       <c r="N27" s="3">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3499,9 +3499,7 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="4">
+      <c r="E28" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="H28" s="13"/>
@@ -3526,8 +3524,7 @@
       <c r="D29" s="13"/>
       <c r="E29" s="4"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="13">
+      <c r="G29" s="13">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I29" s="4"/>
@@ -3551,8 +3548,7 @@
       <c r="D30" s="13"/>
       <c r="E30" s="4"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="13">
+      <c r="G30" s="13">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I30" s="4"/>
@@ -3576,8 +3572,7 @@
       <c r="D31" s="13"/>
       <c r="E31" s="1"/>
       <c r="F31" s="13"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="13">
+      <c r="G31" s="13">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I31" s="1"/>
@@ -3642,7 +3637,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="13"/>
       <c r="E34" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="1"/>
@@ -3654,7 +3649,7 @@
       <c r="M34" s="15"/>
       <c r="N34" s="3">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -3667,7 +3662,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="13"/>
       <c r="E35" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="F35" s="13"/>
       <c r="G35" s="1"/>
@@ -3679,7 +3674,7 @@
       <c r="M35" s="15"/>
       <c r="N35" s="3">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -3733,9 +3728,8 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="24">
-        <v>6.25E-2</v>
+      <c r="E38" s="24">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="H38" s="13"/>
       <c r="I38" s="1"/>
@@ -3745,7 +3739,7 @@
       <c r="M38" s="15"/>
       <c r="N38" s="3">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -3757,11 +3751,10 @@
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="13"/>
-      <c r="E39" s="4"/>
+      <c r="E39" s="24">
+        <v>6.9444444444444434E-2</v>
+      </c>
       <c r="F39" s="13"/>
-      <c r="G39" s="24">
-        <v>6.25E-2</v>
-      </c>
       <c r="H39" s="13"/>
       <c r="I39" s="1"/>
       <c r="J39" s="13"/>
@@ -3770,7 +3763,7 @@
       <c r="M39" s="15"/>
       <c r="N39" s="3">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>6.9444444444444434E-2</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -3876,10 +3869,9 @@
       <c r="D44" s="13"/>
       <c r="E44" s="4"/>
       <c r="F44" s="13"/>
-      <c r="G44" s="24">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="H44" s="13"/>
+      <c r="H44" s="24">
+        <v>0.125</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
@@ -3887,7 +3879,7 @@
       <c r="M44" s="15"/>
       <c r="N44" s="3">
         <f t="shared" si="0"/>
-        <v>0.10416666666666667</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -3901,10 +3893,8 @@
       <c r="D45" s="13"/>
       <c r="E45" s="4"/>
       <c r="F45" s="13"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="4">
-        <v>0.125</v>
+      <c r="H45" s="4">
+        <v>0.10416666666666667</v>
       </c>
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
@@ -3912,7 +3902,7 @@
       <c r="M45" s="15"/>
       <c r="N45" s="3">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -3968,11 +3958,9 @@
       <c r="D48" s="13"/>
       <c r="E48" s="4"/>
       <c r="F48" s="13"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="13">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I48" s="1"/>
+      <c r="I48" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="1"/>
@@ -3995,11 +3983,10 @@
       <c r="F49" s="13"/>
       <c r="G49" s="24"/>
       <c r="H49" s="13"/>
-      <c r="I49" s="1"/>
+      <c r="I49" s="13">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="J49" s="13"/>
-      <c r="L49" s="13">
-        <v>4.1666666666666664E-2</v>
-      </c>
       <c r="M49" s="15"/>
       <c r="N49" s="3">
         <f t="shared" si="0"/>
@@ -4143,7 +4130,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E55" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="F55" s="4">
         <v>2.0833333333333332E-2</v>
@@ -4169,7 +4156,7 @@
       <c r="M55" s="15"/>
       <c r="N55" s="3">
         <f t="shared" si="0"/>
-        <v>0.34722222222222215</v>
+        <v>0.34027777777777773</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -4185,21 +4172,21 @@
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="I56" s="4">
-        <v>0.10416666666666667</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="J56" s="4">
-        <v>0.10416666666666667</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="K56" s="4">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="L56" s="4">
-        <v>4.1666666666666664E-2</v>
+        <v>4.9999999999999996E-2</v>
       </c>
       <c r="M56" s="15"/>
       <c r="N56" s="3">
         <f t="shared" si="0"/>
-        <v>0.33333333333333337</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -4216,7 +4203,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E57" s="4">
-        <v>8.3333333333333329E-2</v>
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="F57" s="4">
         <v>8.3333333333333329E-2</v>
@@ -4242,7 +4229,7 @@
       <c r="M57" s="23"/>
       <c r="N57" s="3">
         <f t="shared" si="0"/>
-        <v>1.125</v>
+        <v>1.0659722222222221</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4285,7 +4272,7 @@
       </c>
       <c r="E59" s="3">
         <f t="shared" si="1"/>
-        <v>0.25416666666666665</v>
+        <v>0.33402777777777776</v>
       </c>
       <c r="F59" s="3">
         <f t="shared" si="1"/>
@@ -4293,7 +4280,7 @@
       </c>
       <c r="G59" s="3">
         <f t="shared" si="1"/>
-        <v>0.32708333333333334</v>
+        <v>0.31666666666666665</v>
       </c>
       <c r="H59" s="3">
         <f t="shared" si="1"/>
@@ -4301,11 +4288,11 @@
       </c>
       <c r="I59" s="3">
         <f>SUM(I2:I58)</f>
-        <v>0.33750000000000002</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="J59" s="3">
         <f>SUM(J2:J58)</f>
-        <v>0.33750000000000002</v>
+        <v>0.25</v>
       </c>
       <c r="K59" s="3">
         <f>SUM(K2:K58)</f>
@@ -4313,7 +4300,7 @@
       </c>
       <c r="L59" s="3">
         <f t="shared" si="1"/>
-        <v>0.30972222222222223</v>
+        <v>0.27638888888888891</v>
       </c>
       <c r="M59" s="3">
         <f t="shared" si="1"/>
@@ -4323,80 +4310,85 @@
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M60" s="3">
         <f>SUM(C59:M59)</f>
-        <v>3.5506944444444448</v>
+        <v>3.4534722222222225</v>
       </c>
       <c r="N60" s="3">
         <f>SUM(N2:N58)</f>
-        <v>3.5506944444444448</v>
+        <v>3.4534722222222216</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N63" s="42"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F54:F56 C52:C58 G52:G58 I52:I53 E52:E58 L52:L58 D57 C28:C50 D32 E25:E50 I25:I50 L25:L48 C25:C26 H54:I55 I56:I58 K56 C2:M7 G25:G37 G39:G50 F38 L50 C13:M24 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12">
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="F54:F56 C52:C58 G52:G58 I52:I53 E52:E58 L52:L58 D57 C28:C50 D32 L25:L48 C25:C26 H54:I55 I56:I58 K56 C2:M7 L50 C13:M20 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12 G25:G26 G32:G37 E25:E50 I25:I44 I46:I47 G40:G43 G46:G47 H44:H45 G49:G50 I21:M22 C21:F24 I50 K23:M24 G23:I24">
+    <cfRule type="cellIs" dxfId="24" priority="16" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:M37 C52:M55 D27:M27 C28:M34 C26:M26 C57:M58 C56:G56 I56:M56 C2:M7 C39:M48 H38:M38 C38:F38 C50:M50 C49:J49 L49:M49 F51:M51 D51 C13:M24 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12">
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
+  <conditionalFormatting sqref="C36:M37 C52:M55 C32:M34 C26:M26 C57:M58 C56:G56 C2:M7 C40:M43 C50:M50 F51:M51 D51 C13:M20 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12 D27:F27 C28:E28 C38:E38 I56:M56 H38:M39 C39:F39 C46:M47 J45:M45 H44:M44 C44:F45 H45 H27:M28 I29:M31 C29:G31 I21:M22 C21:F24 C48:F48 I48:M48 K23:M24 G23:I24 M49 C49:J49">
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51 I51 G51 C51:D51">
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:K57 F57 H57 M57">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54:D56 G54:G56 J54:K55 J56">
     <cfRule type="cellIs" dxfId="19" priority="11" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54:D56 G54:G56 J54:K55 J56">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:M27 C28:M37 C57:M58 C56:G56 I56:M56 C2:M7 C39:M48 H38:M38 C38:F38 C50:M50 C49:J49 L49:M49 C52:M55 F51:M51 C51:D51 C13:M26 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="C32:M37 C57:M58 C56:G56 C2:M7 C40:M43 C50:M50 C52:M55 F51:M51 C51:D51 C13:M20 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12 D27:F27 C28:E28 C38:E38 I56:M56 H38:M39 C39:F39 C46:M47 J45:M45 H44:M44 C44:F45 H45 H27:M28 I29:M31 C29:G31 C25:M26 I21:M22 C48:F48 I48:M48 C21:F24 K23:M24 G23:I24 M49 C49:J49">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N58">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:M59">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>0.333333333333333</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I56">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Creation d'article + affichage + creation commentaire +affichage + afficher tout les articles par topic
</commit_message>
<xml_diff>
--- a/Divers/Planification.xlsx
+++ b/Divers/Planification.xlsx
@@ -1161,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2793,7 @@
   <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3341,7 +3341,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4">
-        <v>2.0833333333333332E-2</v>
+        <v>5.347222222222222E-2</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -3350,7 +3350,7 @@
       <c r="M21" s="23"/>
       <c r="N21" s="3">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>5.347222222222222E-2</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3777,7 +3777,7 @@
       <c r="D40" s="13"/>
       <c r="E40" s="4"/>
       <c r="F40" s="13">
-        <v>8.3333333333333329E-2</v>
+        <v>6.9444444444444434E-2</v>
       </c>
       <c r="G40" s="24"/>
       <c r="H40" s="13"/>
@@ -3788,7 +3788,7 @@
       <c r="M40" s="15"/>
       <c r="N40" s="3">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>6.9444444444444434E-2</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -3802,7 +3802,7 @@
       <c r="D41" s="13"/>
       <c r="E41" s="4"/>
       <c r="F41" s="13">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="G41" s="24"/>
       <c r="H41" s="13"/>
@@ -3813,7 +3813,7 @@
       <c r="M41" s="15"/>
       <c r="N41" s="3">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -4169,7 +4169,9 @@
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
+      <c r="F56" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="G56" s="4"/>
       <c r="I56" s="4">
         <v>9.9999999999999992E-2</v>
@@ -4186,7 +4188,7 @@
       <c r="M56" s="15"/>
       <c r="N56" s="3">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0.35416666666666663</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
@@ -4205,9 +4207,7 @@
       <c r="E57" s="4">
         <v>2.4305555555555556E-2</v>
       </c>
-      <c r="F57" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="F57" s="4"/>
       <c r="G57" s="4">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -4229,7 +4229,7 @@
       <c r="M57" s="23"/>
       <c r="N57" s="3">
         <f t="shared" si="0"/>
-        <v>1.0659722222222221</v>
+        <v>0.98263888888888884</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4276,7 +4276,7 @@
       </c>
       <c r="F59" s="3">
         <f t="shared" si="1"/>
-        <v>0.33749999999999997</v>
+        <v>0.33541666666666659</v>
       </c>
       <c r="G59" s="3">
         <f t="shared" si="1"/>
@@ -4310,11 +4310,11 @@
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M60" s="3">
         <f>SUM(C59:M59)</f>
-        <v>3.4534722222222225</v>
+        <v>3.4513888888888893</v>
       </c>
       <c r="N60" s="3">
         <f>SUM(N2:N58)</f>
-        <v>3.4534722222222216</v>
+        <v>3.4513888888888888</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout de toute les fonctionnalité liée au profile + un peu de refactor de code
</commit_message>
<xml_diff>
--- a/Divers/Planification.xlsx
+++ b/Divers/Planification.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="85">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Creation du GIT</t>
+  </si>
+  <si>
+    <t>Design  du drop down + page profil + page modif profile</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -622,6 +625,34 @@
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2719,67 +2750,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F54:F56 C52:C58 G52:G58 I52:I53 E52:E58 L52:L58 D57 C28:C50 D32 E25:E50 I25:I50 L25:L48 C25:C26 H54:I55 I56:I58 K56 C2:M24 G25:G37 G39:G50 F38 L50">
-    <cfRule type="cellIs" dxfId="39" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="17" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:M37 C52:M55 D27:M27 C28:M34 C26:M26 C57:M58 C56:G56 I56:M56 C2:M24 C39:M48 H38:M38 C38:F38 C50:M50 C49:J49 L49:M49">
-    <cfRule type="cellIs" dxfId="38" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51 I51 G51 E51 C51">
-    <cfRule type="cellIs" dxfId="37" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="15" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:M51">
-    <cfRule type="cellIs" dxfId="36" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:K57 F57 H57 M57">
-    <cfRule type="cellIs" dxfId="35" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54:D56 G54:G56 J54:K55 J56">
-    <cfRule type="cellIs" dxfId="34" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="12" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:M27 C28:M37 C57:M58 C56:G56 I56:M56 C2:M26 C39:M48 H38:M38 C38:F38 C50:M55 C49:J49 L49:M49">
-    <cfRule type="cellIs" dxfId="33" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N58">
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:M59">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2790,10 +2821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,7 +2944,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="23"/>
       <c r="N3" s="3">
-        <f t="shared" ref="N3:N58" si="0">SUM(C3:M3)</f>
+        <f t="shared" ref="N3:N64" si="0">SUM(C3:M3)</f>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -3860,7 +3891,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B44" s="34">
         <v>0.10416666666666667</v>
@@ -3870,7 +3901,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="13"/>
       <c r="H44" s="24">
-        <v>0.125</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="13"/>
@@ -3879,7 +3910,7 @@
       <c r="M44" s="15"/>
       <c r="N44" s="3">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -3958,8 +3989,8 @@
       <c r="D48" s="13"/>
       <c r="E48" s="4"/>
       <c r="F48" s="13"/>
-      <c r="I48" s="13">
-        <v>4.1666666666666664E-2</v>
+      <c r="G48" s="13">
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
@@ -3967,7 +3998,7 @@
       <c r="M48" s="15"/>
       <c r="N48" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -4092,301 +4123,415 @@
         <v>3.472222222222222E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="46" t="s">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="44"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="3"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="44"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="3"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="44"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="3"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="44"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+      <c r="L57" s="13"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="3"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="44"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="13"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="3"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="44"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="3"/>
+    </row>
+    <row r="60" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="B54" s="34">
+      <c r="B60" s="34">
         <f>SUM(B5,B6,B13,B18,B26,B33,B37,B43,B47)</f>
         <v>1.3854166666666665</v>
       </c>
-      <c r="C54" s="50"/>
-      <c r="D54" s="50"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="50"/>
-      <c r="G54" s="50"/>
-      <c r="H54" s="50"/>
-      <c r="I54" s="50"/>
-      <c r="J54" s="50"/>
-      <c r="K54" s="50"/>
-      <c r="L54" s="50"/>
-      <c r="M54" s="52"/>
-      <c r="N54" s="3">
+      <c r="C60" s="50"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="50"/>
+      <c r="H60" s="50"/>
+      <c r="I60" s="50"/>
+      <c r="J60" s="50"/>
+      <c r="K60" s="50"/>
+      <c r="L60" s="50"/>
+      <c r="M60" s="52"/>
+      <c r="N60" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A55" s="46" t="s">
+    <row r="61" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="B55" s="34">
+      <c r="B61" s="34">
         <v>0.36805555555555558</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C61" s="4">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D55" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E55" s="4">
+      <c r="D61" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E61" s="4">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="F55" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G55" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="H55" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="I55" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="J55" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="K55" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="L55" s="4">
+      <c r="F61" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G61" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H61" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="I61" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J61" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="K61" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="L61" s="4">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="M55" s="15"/>
-      <c r="N55" s="3">
+      <c r="M61" s="15"/>
+      <c r="N61" s="3">
         <f t="shared" si="0"/>
         <v>0.34027777777777773</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="46" t="s">
+    <row r="62" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="34">
+      <c r="B62" s="34">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G56" s="4"/>
-      <c r="I56" s="4">
-        <v>9.9999999999999992E-2</v>
-      </c>
-      <c r="J56" s="4">
-        <v>9.9999999999999992E-2</v>
-      </c>
-      <c r="K56" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="L56" s="4">
-        <v>4.9999999999999996E-2</v>
-      </c>
-      <c r="M56" s="15"/>
-      <c r="N56" s="3">
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="I62" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J62" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K62" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L62" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M62" s="15"/>
+      <c r="N62" s="3">
         <f t="shared" si="0"/>
         <v>0.35416666666666663</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="46" t="s">
+    <row r="63" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A63" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B57" s="34">
+      <c r="B63" s="34">
         <v>1.125</v>
       </c>
-      <c r="C57" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D57" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E57" s="4">
+      <c r="C63" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D63" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E63" s="4">
         <v>2.4305555555555556E-2</v>
       </c>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H57" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="I57" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="J57" s="4">
+      <c r="F63" s="4"/>
+      <c r="G63" s="4">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="J63" s="4">
         <v>0.125</v>
       </c>
-      <c r="K57" s="4">
+      <c r="K63" s="4">
         <v>0.20833333333333334</v>
       </c>
-      <c r="L57" s="4">
+      <c r="L63" s="4">
         <v>0.20833333333333334</v>
       </c>
-      <c r="M57" s="23"/>
-      <c r="N57" s="3">
-        <f t="shared" si="0"/>
-        <v>0.98263888888888884</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="47" t="s">
+      <c r="M63" s="23"/>
+      <c r="N63" s="3">
+        <f t="shared" si="0"/>
+        <v>0.89236111111111116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B58" s="37">
+      <c r="B64" s="37">
         <v>0.32916666666666666</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="38"/>
-      <c r="L58" s="6"/>
-      <c r="M58" s="39">
+      <c r="C64" s="2"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="39">
         <v>0.32916666666666666</v>
       </c>
-      <c r="N58" s="3">
+      <c r="N64" s="3">
         <f t="shared" si="0"/>
         <v>0.32916666666666666</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="3">
-        <f>SUM(B2:B3,B54:B58)</f>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B65" s="3">
+        <f>SUM(B2:B3,B60:B64)</f>
         <v>3.6666666666666665</v>
       </c>
-      <c r="C59" s="3">
-        <f t="shared" ref="C59:M59" si="1">SUM(C2:C58)</f>
+      <c r="C65" s="3">
+        <f t="shared" ref="C65:M65" si="1">SUM(C2:C64)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D65" s="3">
         <f t="shared" si="1"/>
         <v>0.3263888888888889</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E65" s="3">
         <f t="shared" si="1"/>
         <v>0.33402777777777776</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F65" s="3">
         <f t="shared" si="1"/>
         <v>0.33541666666666659</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G65" s="3">
         <f t="shared" si="1"/>
+        <v>0.33055555555555555</v>
+      </c>
+      <c r="H65" s="3">
+        <f t="shared" si="1"/>
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="I65" s="3">
+        <f>SUM(I2:I64)</f>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="J65" s="3">
+        <f>SUM(J2:J64)</f>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="K65" s="3">
+        <f>SUM(K2:K64)</f>
         <v>0.31666666666666665</v>
       </c>
-      <c r="H59" s="3">
+      <c r="L65" s="3">
         <f t="shared" si="1"/>
-        <v>0.33749999999999997</v>
-      </c>
-      <c r="I59" s="3">
-        <f>SUM(I2:I58)</f>
-        <v>0.29166666666666663</v>
-      </c>
-      <c r="J59" s="3">
-        <f>SUM(J2:J58)</f>
-        <v>0.25</v>
-      </c>
-      <c r="K59" s="3">
-        <f>SUM(K2:K58)</f>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="L59" s="3">
-        <f t="shared" si="1"/>
-        <v>0.27638888888888891</v>
-      </c>
-      <c r="M59" s="3">
+        <v>0.30972222222222223</v>
+      </c>
+      <c r="M65" s="3">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M60" s="3">
-        <f>SUM(C59:M59)</f>
-        <v>3.4513888888888893</v>
-      </c>
-      <c r="N60" s="3">
-        <f>SUM(N2:N58)</f>
-        <v>3.4513888888888888</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N63" s="42"/>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M66" s="3">
+        <f>SUM(C65:M65)</f>
+        <v>3.4236111111111116</v>
+      </c>
+      <c r="N66" s="3">
+        <f>SUM(N2:N64)</f>
+        <v>3.4236111111111107</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N69" s="42"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F54:F56 C52:C58 G52:G58 I52:I53 E52:E58 L52:L58 D57 C28:C50 D32 L25:L48 C25:C26 H54:I55 I56:I58 K56 C2:M7 L50 C13:M20 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12 G25:G26 G32:G37 E25:E50 I25:I44 I46:I47 G40:G43 G46:G47 H44:H45 G49:G50 I21:M22 C21:F24 I50 K23:M24 G23:I24">
+  <conditionalFormatting sqref="F60:F62 C52:C64 G52:G64 I52:I59 E52:E64 L52:L64 D63 C28:C50 D32 L25:L48 C25:C26 H60:I61 I62:I64 C2:M7 L50 C13:M20 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12 G25:G26 G32:G37 E25:E50 I25:I44 I46:I47 G40:G43 G46:G47 H44:H45 G49:G50 I21:M22 C21:F24 I50 K23:M24 G23:I24 K62:L62">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:M37 C52:M61 C32:M34 C26:M26 C63:M64 C62:G62 C2:M7 C40:M43 C50:M50 F51:M51 D51 C13:M20 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12 D27:F27 C28:E28 C38:E38 H38:M39 C39:F39 C46:M47 J45:M45 H44:M44 C44:F45 H45 H27:M28 I29:M31 C29:G31 I21:M22 C21:F24 K23:M24 G23:I24 M49 C49:J49 J48:M48 C48:G48 I62:M62">
+    <cfRule type="cellIs" dxfId="27" priority="19" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L51 I51 G51 C51:D51">
+    <cfRule type="cellIs" dxfId="26" priority="18" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J63:K63 F63 H63 M63">
     <cfRule type="cellIs" dxfId="24" priority="16" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36:M37 C52:M55 C32:M34 C26:M26 C57:M58 C56:G56 C2:M7 C40:M43 C50:M50 F51:M51 D51 C13:M20 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12 D27:F27 C28:E28 C38:E38 I56:M56 H38:M39 C39:F39 C46:M47 J45:M45 H44:M44 C44:F45 H45 H27:M28 I29:M31 C29:G31 I21:M22 C21:F24 C48:F48 I48:M48 K23:M24 G23:I24 M49 C49:J49">
+  <conditionalFormatting sqref="D60:D62 G60:G62 J60:K61 J62">
     <cfRule type="cellIs" dxfId="23" priority="15" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:M37 C63:M64 C62:G62 C2:M7 C40:M43 C50:M50 C52:M61 F51:M51 C51:D51 C13:M20 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12 D27:F27 C28:E28 C38:E38 H38:M39 C39:F39 C46:M47 J45:M45 H44:M44 C44:F45 H45 H27:M28 I29:M31 C29:G31 C25:M26 I21:M22 C21:F24 K23:M24 G23:I24 M49 C49:J49 J48:M48 C48:G48 I62:M62">
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L51 I51 G51 C51:D51">
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="greaterThan">
+  <conditionalFormatting sqref="N2:N64">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="greaterThan">
+      <formula>$B2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+      <formula>$B2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B65">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="greaterThan">
+      <formula>3.66666666666667</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+      <formula>3.66666666666667</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65:M65">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="greaterThan">
+      <formula>0.333333333333333</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+      <formula>0.333333333333333</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I62">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="21" priority="13" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J57:K57 F57 H57 M57">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="greaterThan">
+  <conditionalFormatting sqref="J62">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54:D56 G54:G56 J54:K55 J56">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="greaterThan">
+  <conditionalFormatting sqref="J62">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:M37 C57:M58 C56:G56 C2:M7 C40:M43 C50:M50 C52:M55 F51:M51 C51:D51 C13:M20 F8:M10 C8:D10 H11:M11 C11:F11 F12:M12 C12:D12 D27:F27 C28:E28 C38:E38 I56:M56 H38:M39 C39:F39 C46:M47 J45:M45 H44:M44 C44:F45 H45 H27:M28 I29:M31 C29:G31 C25:M26 I21:M22 C48:F48 I48:M48 C21:F24 K23:M24 G23:I24 M49 C49:J49">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="greaterThan">
-      <formula>0</formula>
+  <conditionalFormatting sqref="K62">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N58">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
-      <formula>$B2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
-      <formula>$B2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThan">
-      <formula>3.66666666666667</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
-      <formula>3.66666666666667</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:M59">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
-      <formula>0.333333333333333</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
-      <formula>0.333333333333333</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I56">
+  <conditionalFormatting sqref="L62">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>

</xml_diff>

<commit_message>
Creation de la fonctionnalitée qui banni et debanni un utilisateur + creation d'un profil public + privé et j'ai fais en sorte que les articles de l'utilisateur banni ne puisse pas apparaitre
</commit_message>
<xml_diff>
--- a/Divers/Planification.xlsx
+++ b/Divers/Planification.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="86">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -275,7 +275,10 @@
     <t>Creation du GIT</t>
   </si>
   <si>
-    <t>Design  du drop down + page profil + page modif profile</t>
+    <t>Design  du drop down + page profil privé /publique + page modif profile</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur je dois pouvoir supprimer/modifier mes propres commentaires</t>
   </si>
 </sst>
 </file>
@@ -2823,8 +2826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3903,14 +3906,16 @@
       <c r="H44" s="24">
         <v>0.20833333333333334</v>
       </c>
-      <c r="I44" s="1"/>
+      <c r="I44" s="4">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
       <c r="L44" s="1"/>
       <c r="M44" s="15"/>
       <c r="N44" s="3">
         <f t="shared" si="0"/>
-        <v>0.20833333333333334</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -3960,7 +3965,7 @@
       </c>
       <c r="B47" s="34">
         <f>SUM(B48:B53)</f>
-        <v>0.14583333333333334</v>
+        <v>0.18750000000000003</v>
       </c>
       <c r="C47" s="48"/>
       <c r="D47" s="49"/>
@@ -4006,7 +4011,7 @@
         <v>79</v>
       </c>
       <c r="B49" s="34">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="13"/>
@@ -4015,13 +4020,13 @@
       <c r="G49" s="24"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="J49" s="13"/>
       <c r="M49" s="15"/>
       <c r="N49" s="3">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -4124,15 +4129,21 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="34"/>
+      <c r="A54" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="34">
+        <v>1.6666666666666666E-2</v>
+      </c>
       <c r="C54" s="4"/>
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
+      <c r="I54" s="13">
+        <v>1.6666666666666666E-2</v>
+      </c>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
       <c r="L54" s="13"/>
@@ -4225,7 +4236,7 @@
       </c>
       <c r="B60" s="34">
         <f>SUM(B5,B6,B13,B18,B26,B33,B37,B43,B47)</f>
-        <v>1.3854166666666665</v>
+        <v>1.4270833333333333</v>
       </c>
       <c r="C60" s="50"/>
       <c r="D60" s="50"/>
@@ -4343,7 +4354,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="J63" s="4">
-        <v>0.125</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="K63" s="4">
         <v>0.20833333333333334</v>
@@ -4354,7 +4365,7 @@
       <c r="M63" s="23"/>
       <c r="N63" s="3">
         <f t="shared" si="0"/>
-        <v>0.89236111111111116</v>
+        <v>0.97569444444444453</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4385,7 +4396,7 @@
     <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" s="3">
         <f>SUM(B2:B3,B60:B64)</f>
-        <v>3.6666666666666665</v>
+        <v>3.708333333333333</v>
       </c>
       <c r="C65" s="3">
         <f t="shared" ref="C65:M65" si="1">SUM(C2:C64)</f>
@@ -4413,11 +4424,11 @@
       </c>
       <c r="I65" s="3">
         <f>SUM(I2:I64)</f>
-        <v>0.23333333333333334</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J65" s="3">
         <f>SUM(J2:J64)</f>
-        <v>0.23333333333333334</v>
+        <v>0.31666666666666665</v>
       </c>
       <c r="K65" s="3">
         <f>SUM(K2:K64)</f>
@@ -4435,11 +4446,11 @@
     <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="M66" s="3">
         <f>SUM(C65:M65)</f>
-        <v>3.4236111111111116</v>
+        <v>3.6069444444444443</v>
       </c>
       <c r="N66" s="3">
         <f>SUM(N2:N64)</f>
-        <v>3.4236111111111107</v>
+        <v>3.5902777777777777</v>
       </c>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.25">

</xml_diff>